<commit_message>
steps towards working mvp
</commit_message>
<xml_diff>
--- a/data/01_input/03_building_devs/Devs.xlsx
+++ b/data/01_input/03_building_devs/Devs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\deq_demonstrator\data\01_input\03_building_devs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1AB4D68-978B-4138-B773-2E5DD86722BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A47D7CE0-FEB7-41C7-9811-76E6BCAD2BD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31740" yWindow="2940" windowWidth="21600" windowHeight="11265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5850" yWindow="4545" windowWidth="16800" windowHeight="5175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Quartier" sheetId="1" r:id="rId1"/>
@@ -425,17 +425,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="16" width="11.42578125" customWidth="1"/>
+    <col min="2" max="16" width="11.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -494,7 +494,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
@@ -553,7 +553,7 @@
         <v>16938</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
@@ -606,13 +606,13 @@
         <v>9959</v>
       </c>
       <c r="R3">
-        <v>2553</v>
+        <v>10000</v>
       </c>
       <c r="S3">
         <v>17797</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
@@ -665,13 +665,13 @@
         <v>7269</v>
       </c>
       <c r="R4">
-        <v>1929</v>
+        <v>10000</v>
       </c>
       <c r="S4">
         <v>13084</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>3</v>
       </c>
@@ -724,13 +724,13 @@
         <v>7532</v>
       </c>
       <c r="R5">
-        <v>1990</v>
+        <v>10000</v>
       </c>
       <c r="S5">
         <v>13545</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>4</v>
       </c>
@@ -789,13 +789,13 @@
         <v>52489</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
     </row>
-    <row r="10" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>